<commit_message>
add interactive scenario between java client and cldr pattern
</commit_message>
<xml_diff>
--- a/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
+++ b/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480D838-E1E1-4F55-9514-F91D44EFF9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F939D278-CD73-43BE-864B-BA26BAE93B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$29</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="126">
   <si>
     <t>Case Name</t>
   </si>
@@ -369,6 +372,48 @@
   </si>
   <si>
     <t>main.zh-Hans.localeDisplayNames.localeDisplayPattern.localePattern</t>
+  </si>
+  <si>
+    <t>CLDRJar</t>
+  </si>
+  <si>
+    <t>Check the number data can be fetched</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Il y a 100 000 fichiers sur "MyDisk".</t>
+  </si>
+  <si>
+    <t>Check the percent data can be fetched</t>
+  </si>
+  <si>
+    <t>Check the plurals data can be fetched</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>plural</t>
+  </si>
+  <si>
+    <t>Check the datetime data can be fetched</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Check the currency data can be fetched</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>US$201,703.54</t>
+  </si>
+  <si>
+    <t>2017年11月20日 GMT+8 下午1:39:24</t>
   </si>
 </sst>
 </file>
@@ -420,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -429,6 +474,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -745,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.05078125" defaultRowHeight="14.4"/>
@@ -1453,7 +1504,93 @@
         <v>21</v>
       </c>
     </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="4">
+        <v>201703.54199999999</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H29" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add interactive scenario with java client
</commit_message>
<xml_diff>
--- a/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
+++ b/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480D838-E1E1-4F55-9514-F91D44EFF9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F939D278-CD73-43BE-864B-BA26BAE93B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$29</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="126">
   <si>
     <t>Case Name</t>
   </si>
@@ -369,6 +372,48 @@
   </si>
   <si>
     <t>main.zh-Hans.localeDisplayNames.localeDisplayPattern.localePattern</t>
+  </si>
+  <si>
+    <t>CLDRJar</t>
+  </si>
+  <si>
+    <t>Check the number data can be fetched</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Il y a 100 000 fichiers sur "MyDisk".</t>
+  </si>
+  <si>
+    <t>Check the percent data can be fetched</t>
+  </si>
+  <si>
+    <t>Check the plurals data can be fetched</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>plural</t>
+  </si>
+  <si>
+    <t>Check the datetime data can be fetched</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Check the currency data can be fetched</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>US$201,703.54</t>
+  </si>
+  <si>
+    <t>2017年11月20日 GMT+8 下午1:39:24</t>
   </si>
 </sst>
 </file>
@@ -420,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -429,6 +474,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -745,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.05078125" defaultRowHeight="14.4"/>
@@ -1453,7 +1504,93 @@
         <v>21</v>
       </c>
     </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="4">
+        <v>201703.54199999999</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H29" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update the test data since timezone is different
</commit_message>
<xml_diff>
--- a/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
+++ b/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\SmokeTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepository\github\MyForked\new\singleton\autotest\cldrpattern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F939D278-CD73-43BE-864B-BA26BAE93B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC6B51-D3D1-4B7F-B767-8412ADA24464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
     <t>US$201,703.54</t>
   </si>
   <si>
-    <t>2017年11月20日 GMT+8 下午1:39:24</t>
+    <t>2017年11月20日 GMT+0 上午5:39:24</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.05078125" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
add file directory structure check
</commit_message>
<xml_diff>
--- a/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
+++ b/autotest/cldrpattern/ExtractedPatternLibTestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepository\github\MyForked\new\singleton\autotest\cldrpattern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\SmokeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC6B51-D3D1-4B7F-B767-8412ADA24464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4F1A4C-8ED3-4128-94F8-57EA9CAF7FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{AB6A95A3-9E40-40A1-8C7F-B7F1A0E15C04}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="223">
   <si>
     <t>Case Name</t>
   </si>
@@ -53,9 +53,6 @@
     <t>2.检查某个文件里的某项数据</t>
   </si>
   <si>
-    <t>3.检查一共有多少个文件</t>
-  </si>
-  <si>
     <t>阿法尔语</t>
   </si>
   <si>
@@ -413,20 +410,321 @@
     <t>US$201,703.54</t>
   </si>
   <si>
-    <t>2017年11月20日 GMT+0 上午5:39:24</t>
+    <t>2017年11月20日 GMT+8 下午1:39:24</t>
+  </si>
+  <si>
+    <t>Check the content in en language folder: cities.json</t>
+  </si>
+  <si>
+    <t>/cities.json</t>
+  </si>
+  <si>
+    <t>PureJsonValueCheck</t>
+  </si>
+  <si>
+    <t>./src/main/resources/cldr/localedata/en</t>
+  </si>
+  <si>
+    <t>cities.AG</t>
+  </si>
+  <si>
+    <t>[{'geonameid': '3576022', 'name': 'Saint John’s', 'translatedname': 'Saint John’s', 'lat': '17.11717', 'lng': '-61.84573'}]</t>
+  </si>
+  <si>
+    <t>File Source</t>
+  </si>
+  <si>
+    <t>jar</t>
+  </si>
+  <si>
+    <t>Check the number of folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the file name in folder:  aliases </t>
+  </si>
+  <si>
+    <t>['aliases.json']</t>
+  </si>
+  <si>
+    <t>languageAlias.zh-CN</t>
+  </si>
+  <si>
+    <t>Check the content in file: aliases.json</t>
+  </si>
+  <si>
+    <t>Check the file name in folder:  core</t>
+  </si>
+  <si>
+    <t>Check the content in file: parse.json</t>
+  </si>
+  <si>
+    <t>/parse.json</t>
+  </si>
+  <si>
+    <t>en-Latn-US</t>
+  </si>
+  <si>
+    <t>likelySubtag.en</t>
+  </si>
+  <si>
+    <t>Check the file name in folder: defaultContent</t>
+  </si>
+  <si>
+    <t>Check the content in file: defaultContent.json</t>
+  </si>
+  <si>
+    <t>/defaultContent.json</t>
+  </si>
+  <si>
+    <t>defaultContent.ky-kg</t>
+  </si>
+  <si>
+    <t>ky-KG</t>
+  </si>
+  <si>
+    <t>Check the number of locales in folder: localedata</t>
+  </si>
+  <si>
+    <t>Check special locale is in localedata folder: root</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>FolderNameCheck</t>
+  </si>
+  <si>
+    <t>{'_reason': 'legacy', '_replacement': 'zh-Hans-CN'}</t>
+  </si>
+  <si>
+    <t>['parse.json']</t>
+  </si>
+  <si>
+    <t>['defaultContent.json']</t>
+  </si>
+  <si>
+    <t>Check the file names are correct in each locale folder</t>
+  </si>
+  <si>
+    <t>Check the file names are correct in each locale(except en) folder</t>
+  </si>
+  <si>
+    <t>LocaleFileNameCheck</t>
+  </si>
+  <si>
+    <t>['languages.json', 'localeDisplayNames.json', 'scripts.json', 'territories.json', 'variants.json']</t>
+  </si>
+  <si>
+    <t>cldr/localedata</t>
+  </si>
+  <si>
+    <t>cldr/localedata/en</t>
+  </si>
+  <si>
+    <t>Check the number of files in folder: localedata</t>
+  </si>
+  <si>
+    <t>LocaleFileCountCheck</t>
+  </si>
+  <si>
+    <t>cldr/defaultContent</t>
+  </si>
+  <si>
+    <t>cldr/aliases</t>
+  </si>
+  <si>
+    <t>cldr/core</t>
+  </si>
+  <si>
+    <t>cldr</t>
+  </si>
+  <si>
+    <t>Check the content in file: cities.json</t>
+  </si>
+  <si>
+    <t>Check the number of locales in folder: misc</t>
+  </si>
+  <si>
+    <t>cldr/misc</t>
+  </si>
+  <si>
+    <t>['contextTransforms.json']</t>
+  </si>
+  <si>
+    <t>Check the number of files in folder: misc</t>
+  </si>
+  <si>
+    <t>Check the content in file: contextTransforms.json</t>
+  </si>
+  <si>
+    <t>cldr/misc/en-150</t>
+  </si>
+  <si>
+    <t>Check the number of folder in folder: pattern</t>
+  </si>
+  <si>
+    <t>Check the number of locales in folder: common</t>
+  </si>
+  <si>
+    <t>cldr/pattern</t>
+  </si>
+  <si>
+    <t>cldr/pattern/common</t>
+  </si>
+  <si>
+    <t>['dateFields.json', 'pattern.json']</t>
+  </si>
+  <si>
+    <t>Check the number of files in folder: common</t>
+  </si>
+  <si>
+    <t>Check the content in file: dateFields.json</t>
+  </si>
+  <si>
+    <t>Check the content in file: pattern.json</t>
+  </si>
+  <si>
+    <t>/pattern.json</t>
+  </si>
+  <si>
+    <t>cldr/pattern/common/pt-MZ</t>
+  </si>
+  <si>
+    <t>dateFields.year.relativeTime-type-future.relativeTimePattern-count-other</t>
+  </si>
+  <si>
+    <t>dentro de {0} anos</t>
+  </si>
+  <si>
+    <t>Check the number of locales in folder: timezone</t>
+  </si>
+  <si>
+    <t>cldr/pattern/timezone</t>
+  </si>
+  <si>
+    <t>['timeZoneName.json']</t>
+  </si>
+  <si>
+    <t>/timeZoneName.json</t>
+  </si>
+  <si>
+    <t>timeZoneNames.gmtFormat</t>
+  </si>
+  <si>
+    <t>UTC{0}</t>
+  </si>
+  <si>
+    <t>cldr/pattern/timezone/fr</t>
+  </si>
+  <si>
+    <t>Check the file name in folder: plurals</t>
+  </si>
+  <si>
+    <t>Check the content in file: plurals.json</t>
+  </si>
+  <si>
+    <t>cldr/plurals</t>
+  </si>
+  <si>
+    <t>['plurals.json']</t>
+  </si>
+  <si>
+    <t>pluralInfo.ak.pluralRule-count-one</t>
+  </si>
+  <si>
+    <t>Check the file name in folder: regionLanguage</t>
+  </si>
+  <si>
+    <t>Check the content in file: regionLanguageMapping.json</t>
+  </si>
+  <si>
+    <t>cldr/regionLanguage</t>
+  </si>
+  <si>
+    <t>/regionLanguageMapping.json</t>
+  </si>
+  <si>
+    <t>['regionLanguageMapping.json']</t>
+  </si>
+  <si>
+    <t>regionInfo.AD</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>Check the file name in folder: supplement</t>
+  </si>
+  <si>
+    <t>cldr/supplement</t>
+  </si>
+  <si>
+    <t>['currencies.json', 'dates.json', 'languageData.json', 'numbers.json']</t>
+  </si>
+  <si>
+    <t>Check the content in file: currencies.json</t>
+  </si>
+  <si>
+    <t>fractions.ALL</t>
+  </si>
+  <si>
+    <t>/dates.json</t>
+  </si>
+  <si>
+    <t>dayPeriodRuleSet.af.afternoon1._from</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>Check the content in file: languageData.json</t>
+  </si>
+  <si>
+    <t>Check the content in file: dates.json</t>
+  </si>
+  <si>
+    <t>languageData.aa._scripts</t>
+  </si>
+  <si>
+    <t>Check the content in file: numbers.json</t>
+  </si>
+  <si>
+    <t>numberingSystems.armn._rules</t>
+  </si>
+  <si>
+    <t>{'_rounding': '0', '_digits': '0'}</t>
+  </si>
+  <si>
+    <t>contextTransforms.relative.stand-alone</t>
+  </si>
+  <si>
+    <t>categories.dates.dayPeriodsFormat.narrow</t>
+  </si>
+  <si>
+    <t>['a.m.', 'p.m.', 'meia-noite', 'meio-dia', 'manhã', 'tarde', 'noite', 'madrugada']</t>
+  </si>
+  <si>
+    <t>['cities.json']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,21 +763,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -796,32 +1100,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="39.05078125" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6.9453125" style="1" customWidth="1"/>
     <col min="2" max="3" width="39.05078125" style="1"/>
-    <col min="4" max="4" width="48.3125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="39.05078125" style="1"/>
+    <col min="4" max="4" width="28.89453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.26171875" style="1" customWidth="1"/>
+    <col min="6" max="8" width="39.05078125" style="1"/>
+    <col min="9" max="9" width="6.7890625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="39.05078125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -830,10 +1137,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1">
@@ -841,19 +1151,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="3">
         <v>27</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.8">
@@ -861,25 +1171,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="28.8">
@@ -887,25 +1197,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="34.799999999999997" customHeight="1">
@@ -913,25 +1223,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="28.8">
@@ -939,25 +1249,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="28.8">
@@ -965,25 +1275,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="28.8">
@@ -991,25 +1301,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="3" customFormat="1" ht="28.8">
@@ -1017,19 +1327,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="3">
         <v>523</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="28.8">
@@ -1037,25 +1347,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="28.8">
@@ -1063,25 +1373,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="28.8">
@@ -1089,25 +1399,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1115,19 +1425,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="1">
         <v>4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="28.8">
@@ -1135,19 +1445,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G14" s="1">
         <v>523</v>
       </c>
       <c r="H14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="28.8">
@@ -1155,25 +1465,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>3</v>
@@ -1184,413 +1494,1220 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="28.8" customHeight="1">
+    <row r="17" spans="1:8" ht="28.8" customHeight="1">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="30.6" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30.6" customHeight="1">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="32.4" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="32.4" customHeight="1">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G19" s="1">
         <v>5</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="28.8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.8">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G20" s="1">
         <v>523</v>
       </c>
       <c r="H20" t="s">
-        <v>20</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="30.6" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30.6" customHeight="1">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="31.2" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="31.2" customHeight="1">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G22" s="1">
         <v>6</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="31.2" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="31.2" customHeight="1">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G23" s="1">
         <v>523</v>
       </c>
       <c r="H23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="31.2" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="31.2" customHeight="1">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="31.2" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="31.2" customHeight="1">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="31.2" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="31.2" customHeight="1">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G26" s="1">
         <v>523</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="31.2" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="31.2" customHeight="1">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="31.2" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="31.2" customHeight="1">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G28" s="1">
         <v>2</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="31.2" customHeight="1">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="G30" t="s">
         <v>79</v>
       </c>
-      <c r="G29" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="G31" s="4">
+        <v>201703.54199999999</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G30" s="4">
-        <v>201703.54199999999</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0.23</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="H33" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>124</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" s="1">
+        <v>9</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.8">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="3">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="28.8">
+      <c r="A43" s="3">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="1">
+        <v>523</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="3">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28.8">
+      <c r="A45" s="3">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2616</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="43.2">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G48" s="1">
+        <v>228</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="28.8">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" s="1">
+        <v>228</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="28.8">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G53" s="1">
+        <v>523</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="28.8">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G55" s="1">
+        <v>1046</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="28.8">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="28.8">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G58" s="1">
+        <v>523</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="28.8">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="1">
+        <v>523</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="28.8">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="28.8">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="28.8">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="3">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="3">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="3">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H29" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}"/>
+  <autoFilter ref="A1:H30" xr:uid="{AB6CEFA1-DB28-4C75-A8F0-CF956BB87EB7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>